<commit_message>
Now draws a barrel object in the scene
Used Obj2Header.exe to convert barrel obj into header and loaded it into my scene.

Updated rubric as well
</commit_message>
<xml_diff>
--- a/ddepewRubric.xlsx
+++ b/ddepewRubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{7B083A0D-A098-450A-BF6E-0DFE594829D5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{CCC188FE-97E3-456D-8A9F-B7A2D5BAEC82}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-465" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="100">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -911,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1026,11 +1026,15 @@
       <c r="D4" s="5">
         <v>2</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="3"/>
+      <c r="E4" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="G4" s="16">
         <f t="shared" ref="G4:G68" si="0" xml:space="preserve"> IF(EXACT(F4,"X"),IF(EXACT(E4,"I"),$B4,IF(EXACT(E4,"II"),$C4,IF(EXACT(E4,"III"),$D4,0))),0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H4" s="17">
         <f>IF(SUMIF(E4:E84,"=I",G4:G84) + SUMIF(C86:C87, "X",B86:B87) &gt; 18, 18, SUMIF(E4:E84,"=I",G4:G84) + SUMIF(C86:C87, "X",B86:B87))</f>
@@ -1038,7 +1042,7 @@
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E84,"=II",G4:G84) + SUMIF(D86:D87, "X",B86:B87) &gt; 18, 18, SUMIF(E4:E84,"=II",G4:G84) + SUMIF(D86:D87, "X",B86:B87))</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E84,"=III",G4:G84) + SUMIF(E86:E87, "X",B86:B87) &gt; 18, 18, SUMIF(E4:E84,"=III",G4:G84) + SUMIF(E86:E87, "X",B86:B87))</f>
@@ -1050,7 +1054,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G84) + SUMIF(C86:C87, "X",B86:B87) + SUMIF(D86:D87, "X",B86:B87) + SUMIF(E86:E87, "X",B86:B87)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1167,7 +1171,9 @@
       <c r="D8" s="5">
         <v>1</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="F8" s="3"/>
       <c r="G8" s="16">
         <f t="shared" si="0"/>
@@ -1179,7 +1185,7 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
@@ -1846,7 +1852,9 @@
       <c r="D37" s="5">
         <v>1</v>
       </c>
-      <c r="E37" s="2"/>
+      <c r="E37" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="F37" s="3"/>
       <c r="G37" s="16">
         <f t="shared" si="0"/>
@@ -3091,7 +3099,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Updated barrel texture + Rubric updated
Barrel now uses its proper texture

Rubric updated for points
</commit_message>
<xml_diff>
--- a/ddepewRubric.xlsx
+++ b/ddepewRubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{CCC188FE-97E3-456D-8A9F-B7A2D5BAEC82}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{4E3FC42E-F001-4BB6-B475-0810B8616CB6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-465" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="100">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -911,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,11 +1038,11 @@
       </c>
       <c r="H4" s="17">
         <f>IF(SUMIF(E4:E84,"=I",G4:G84) + SUMIF(C86:C87, "X",B86:B87) &gt; 18, 18, SUMIF(E4:E84,"=I",G4:G84) + SUMIF(C86:C87, "X",B86:B87))</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E84,"=II",G4:G84) + SUMIF(D86:D87, "X",B86:B87) &gt; 18, 18, SUMIF(E4:E84,"=II",G4:G84) + SUMIF(D86:D87, "X",B86:B87))</f>
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E84,"=III",G4:G84) + SUMIF(E86:E87, "X",B86:B87) &gt; 18, 18, SUMIF(E4:E84,"=III",G4:G84) + SUMIF(E86:E87, "X",B86:B87))</f>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G84) + SUMIF(C86:C87, "X",B86:B87) + SUMIF(D86:D87, "X",B86:B87) + SUMIF(E86:E87, "X",B86:B87)</f>
-        <v>9</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1174,18 +1174,20 @@
       <c r="E8" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="G8" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 18, IF(K4+H4 &gt; 18, 18- H4, K4),0)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
@@ -1489,10 +1491,12 @@
       <c r="E21" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F21" s="3"/>
+      <c r="F21" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="G21" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -1855,10 +1859,12 @@
       <c r="E37" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F37" s="3"/>
+      <c r="F37" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="G37" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
@@ -2321,10 +2327,12 @@
       <c r="E57" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F57" s="3"/>
+      <c r="F57" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="G57" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
@@ -2451,10 +2459,12 @@
       <c r="E63" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F63" s="3"/>
+      <c r="F63" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="G63" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
@@ -2478,10 +2488,12 @@
       <c r="E64" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F64" s="3"/>
+      <c r="F64" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="G64" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
@@ -2505,10 +2517,12 @@
       <c r="E65" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F65" s="3"/>
+      <c r="F65" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="G65" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
@@ -3099,7 +3113,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Updated rubric for points
</commit_message>
<xml_diff>
--- a/ddepewRubric.xlsx
+++ b/ddepewRubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{003A11CC-40E8-413A-AF13-8D1B6773DFF8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{66549CBE-B5E4-428E-9B06-6F3AD73D15BC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-465" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="101">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -915,7 +915,7 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,7 +1108,9 @@
       <c r="D6" s="5">
         <v>4</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="F6" s="3"/>
       <c r="G6" s="16">
         <f t="shared" si="0"/>
@@ -3120,7 +3122,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
MSAA and fixed camera controls
MSAA added to lines and camera now is same speed regardless of window size
</commit_message>
<xml_diff>
--- a/ddepewRubric.xlsx
+++ b/ddepewRubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{66549CBE-B5E4-428E-9B06-6F3AD73D15BC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{861F7F86-09F3-4291-9D8F-5EF3B0654DD9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-465" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="101">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -914,8 +914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,7 +1049,7 @@
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E84,"=III",G4:G84) + SUMIF(E86:E87, "X",B86:B87) &gt; 18, 18, SUMIF(E4:E84,"=III",G4:G84) + SUMIF(E86:E87, "X",B86:B87))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
@@ -1057,7 +1057,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G84) + SUMIF(C86:C87, "X",B86:B87) + SUMIF(D86:D87, "X",B86:B87) + SUMIF(E86:E87, "X",B86:B87)</f>
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1198,7 +1198,7 @@
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1249,7 +1249,9 @@
       <c r="D10" s="5">
         <v>1</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="F10" s="3"/>
       <c r="G10" s="16">
         <f t="shared" si="0"/>
@@ -2308,7 +2310,9 @@
       <c r="D56" s="5">
         <v>2</v>
       </c>
-      <c r="E56" s="2"/>
+      <c r="E56" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="F56" s="3"/>
       <c r="G56" s="16">
         <f t="shared" si="0"/>
@@ -2967,7 +2971,9 @@
       <c r="D86" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E86" s="3"/>
+      <c r="E86" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="F86" s="5"/>
       <c r="G86" s="5"/>
       <c r="H86" s="5"/>
@@ -2989,7 +2995,9 @@
       <c r="D87" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E87" s="3"/>
+      <c r="E87" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="F87" s="5"/>
       <c r="G87" s="5"/>
       <c r="H87" s="5"/>
@@ -3122,7 +3130,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Updated model loader to work with textures
Rubric also updated
</commit_message>
<xml_diff>
--- a/ddepewRubric.xlsx
+++ b/ddepewRubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{861F7F86-09F3-4291-9D8F-5EF3B0654DD9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{5D8D9601-9D24-407B-B61F-7BB0AB1C28DF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-465" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="101">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -914,8 +914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,7 +1049,7 @@
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E84,"=III",G4:G84) + SUMIF(E86:E87, "X",B86:B87) &gt; 18, 18, SUMIF(E4:E84,"=III",G4:G84) + SUMIF(E86:E87, "X",B86:B87))</f>
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
@@ -1057,7 +1057,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G84) + SUMIF(C86:C87, "X",B86:B87) + SUMIF(D86:D87, "X",B86:B87) + SUMIF(E86:E87, "X",B86:B87)</f>
-        <v>23</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1076,10 +1076,12 @@
       <c r="E5" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="G5" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>27</v>
@@ -1111,10 +1113,12 @@
       <c r="E6" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="G6" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H6" s="17">
         <f>IF(SUMIF(E4:E84,"=I",G4:G84) + SUMIF(C86:C87, "X",B86:B87)  &gt; 18, SUMIF(E4:E84,"=I",G4:G84) + SUMIF(C86:C87, "X",B86:B87) - 18,0)</f>
@@ -1198,7 +1202,7 @@
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1219,10 +1223,12 @@
       <c r="E9" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="G9" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="19" t="s">
         <v>26</v>
@@ -1252,10 +1258,12 @@
       <c r="E10" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F10" s="3"/>
+      <c r="F10" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="G10" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 18 &gt; 0, K4+H4 - 18, 0)</f>
@@ -1921,11 +1929,15 @@
       <c r="D39" s="5">
         <v>4</v>
       </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="3"/>
+      <c r="E39" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="G39" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
@@ -2313,10 +2325,12 @@
       <c r="E56" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F56" s="3"/>
+      <c r="F56" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="G56" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
@@ -3130,7 +3144,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Fixed instancing to work with my array system
</commit_message>
<xml_diff>
--- a/ddepewRubric.xlsx
+++ b/ddepewRubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7704B402-7E73-4CE7-81D6-860E835EE5D8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{64BCD3D7-64BD-47C6-A7A1-81EEEA6E2826}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-465" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="99">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -908,8 +908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1954,7 +1954,9 @@
       <c r="D40" s="5">
         <v>3</v>
       </c>
-      <c r="E40" s="2"/>
+      <c r="E40" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="F40" s="3"/>
       <c r="G40" s="16">
         <f t="shared" si="0"/>
@@ -3132,7 +3134,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Implemented basic normal mapping on a cube
Also updated rubric for final points for milestone 1
</commit_message>
<xml_diff>
--- a/ddepewRubric.xlsx
+++ b/ddepewRubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{47984505-01B4-4FBE-B1F5-38B046FA0751}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C3F6FC5E-74D5-417A-A07D-A4B569AC20A4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-465" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="99">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -908,8 +908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,11 +1047,11 @@
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G84) + SUMIF(C86:C87, "X",B86:B87) + SUMIF(D86:D87, "X",B86:B87) + SUMIF(E86:E87, "X",B86:B87)</f>
-        <v>36</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1116,7 +1116,7 @@
       </c>
       <c r="H6" s="17">
         <f>IF(SUMIF(E4:E84,"=I",G4:G84) + SUMIF(C86:C87, "X",B86:B87)  &gt; 18, SUMIF(E4:E84,"=I",G4:G84) + SUMIF(C86:C87, "X",B86:B87) - 18,0)</f>
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="I6" s="17">
         <f>IF(SUMIF(E4:E84,"=II",G4:G84) + SUMIF(D86:D87, "X",B86:B87) &gt; 18, SUMIF(E4:E84,"=II",G4:G84) + SUMIF(D86:D87, "X",B86:B87) - 18,0)</f>
@@ -1196,7 +1196,7 @@
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1261,11 +1261,11 @@
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 18 &gt; 0, K4+H4 - 18, 0)</f>
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 18 &gt; 0, H10+I4 - 18, 0)</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="J10" s="19">
         <f>IF(I10+J4 - 18 &gt; 0, I10+J4 - 18, 0)</f>
@@ -1362,11 +1362,15 @@
       <c r="D14" s="5">
         <v>4</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="3"/>
+      <c r="E14" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="G14" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -1533,10 +1537,12 @@
       <c r="E22" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F22" s="3"/>
+      <c r="F22" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="G22" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
@@ -1560,10 +1566,12 @@
       <c r="E23" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F23" s="3"/>
+      <c r="F23" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="G23" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
@@ -1587,10 +1595,12 @@
       <c r="E24" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F24" s="3"/>
+      <c r="F24" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="G24" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
@@ -1961,10 +1971,12 @@
       <c r="E40" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F40" s="3"/>
+      <c r="F40" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="G40" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
@@ -3138,7 +3150,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Small change to LoadOBJ to reduce wasted memory
</commit_message>
<xml_diff>
--- a/ddepewRubric.xlsx
+++ b/ddepewRubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C3F6FC5E-74D5-417A-A07D-A4B569AC20A4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3123CEB0-5EF4-4864-A8C7-31B0556E61E9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-465" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="100">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -319,6 +319,9 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>II</t>
   </si>
 </sst>
 </file>
@@ -908,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1145,7 +1148,9 @@
       <c r="D7" s="5">
         <v>1</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="F7" s="3"/>
       <c r="G7" s="16">
         <f t="shared" si="0"/>
@@ -3150,7 +3155,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Second viewport implemented + Specular work started
Second viewport now renders alongside the first one, it's basically splitscreen with different views of the same scene.

Specular work was started as well in the Master_PS and VS

+ Rubric updates for viewport
</commit_message>
<xml_diff>
--- a/ddepewRubric.xlsx
+++ b/ddepewRubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3123CEB0-5EF4-4864-A8C7-31B0556E61E9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BDD8EF1A-F7B1-4A08-94D0-ABDE416F57F7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-465" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="100">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -911,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1042,7 +1042,7 @@
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E84,"=II",G4:G84) + SUMIF(D86:D87, "X",B86:B87) &gt; 18, 18, SUMIF(E4:E84,"=II",G4:G84) + SUMIF(D86:D87, "X",B86:B87))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E84,"=III",G4:G84) + SUMIF(E86:E87, "X",B86:B87) &gt; 18, 18, SUMIF(E4:E84,"=III",G4:G84) + SUMIF(E86:E87, "X",B86:B87))</f>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G84) + SUMIF(C86:C87, "X",B86:B87) + SUMIF(D86:D87, "X",B86:B87) + SUMIF(E86:E87, "X",B86:B87)</f>
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1132,7 +1132,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="15">
         <f>IF(L4 &gt; 54, SUM(-54,L4),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1151,10 +1151,12 @@
       <c r="E7" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="G7" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>23</v>
@@ -1201,7 +1203,7 @@
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1270,11 +1272,11 @@
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 18 &gt; 0, H10+I4 - 18, 0)</f>
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="J10" s="19">
         <f>IF(I10+J4 - 18 &gt; 0, I10+J4 - 18, 0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -2639,11 +2641,15 @@
       <c r="D68" s="5">
         <v>4</v>
       </c>
-      <c r="E68" s="2"/>
-      <c r="F68" s="3"/>
+      <c r="E68" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="G68" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
@@ -3155,7 +3161,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Some misc changes to lighting to better see the specular on the cube
</commit_message>
<xml_diff>
--- a/ddepewRubric.xlsx
+++ b/ddepewRubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{198A75FC-EF03-47F4-AA57-FFE127A258EA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F90A9B1A-833D-41CA-BDB1-CADE34545C3A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-465" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -911,7 +911,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -3169,7 +3169,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Updated rubric + readme
</commit_message>
<xml_diff>
--- a/ddepewRubric.xlsx
+++ b/ddepewRubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F90A9B1A-833D-41CA-BDB1-CADE34545C3A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A9EEAD43-1CF9-46C0-B365-A5ECD174AF3B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-465" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="101">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -322,6 +322,9 @@
   </si>
   <si>
     <t>II</t>
+  </si>
+  <si>
+    <t>III</t>
   </si>
 </sst>
 </file>
@@ -912,7 +915,7 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,7 +1049,7 @@
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E84,"=III",G4:G84) + SUMIF(E86:E87, "X",B86:B87) &gt; 18, 18, SUMIF(E4:E84,"=III",G4:G84) + SUMIF(E86:E87, "X",B86:B87))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
@@ -1054,7 +1057,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G84) + SUMIF(C86:C87, "X",B86:B87) + SUMIF(D86:D87, "X",B86:B87) + SUMIF(E86:E87, "X",B86:B87)</f>
-        <v>63</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1132,7 +1135,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="15">
         <f>IF(L4 &gt; 54, SUM(-54,L4),0)</f>
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1276,7 +1279,7 @@
       </c>
       <c r="J10" s="19">
         <f>IF(I10+J4 - 18 &gt; 0, I10+J4 - 18, 0)</f>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -2868,11 +2871,15 @@
       <c r="D79" s="5">
         <v>4</v>
       </c>
-      <c r="E79" s="2"/>
-      <c r="F79" s="3"/>
+      <c r="E79" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="G79" s="16">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H79" s="5"/>
       <c r="I79" s="5"/>
@@ -3014,7 +3021,9 @@
       <c r="D86" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E86" s="3"/>
+      <c r="E86" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="F86" s="5"/>
       <c r="G86" s="5"/>
       <c r="H86" s="5"/>
@@ -3036,7 +3045,9 @@
       <c r="D87" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E87" s="3"/>
+      <c r="E87" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="F87" s="5"/>
       <c r="G87" s="5"/>
       <c r="H87" s="5"/>
@@ -3169,7 +3180,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>